<commit_message>
Adding Summary / Detail Reports.
</commit_message>
<xml_diff>
--- a/source/Databases/NxseSales/PAYROLL/REPORTS/PayPeriod -- 002.xlsx
+++ b/source/Databases/NxseSales/PAYROLL/REPORTS/PayPeriod -- 002.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26310" windowHeight="12360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26310" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -261,9 +261,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>AdjustmentAmount</t>
-  </si>
-  <si>
     <t>CreatedOn</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>Total Pay</t>
+  </si>
+  <si>
+    <t>Adj Amount</t>
   </si>
 </sst>
 </file>
@@ -291,8 +291,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -318,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,6 +340,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,39 +389,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -699,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -744,1154 +747,1154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
         <v>42099.25</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="5">
         <v>42106.25</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="4">
         <v>191186</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="4">
         <v>3091516</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="5">
         <v>42089.426510219906</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="5">
         <v>42089.444309456019</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="8">
+      <c r="O2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="5">
         <v>42101.033493668983</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="8">
+      <c r="Q2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="5">
         <v>42104.033493668983</v>
       </c>
-      <c r="S2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="7">
+      <c r="S2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="4">
         <v>3</v>
       </c>
-      <c r="V2" s="7">
+      <c r="V2" s="4">
         <v>5000</v>
       </c>
-      <c r="W2" s="7">
-        <v>0</v>
-      </c>
-      <c r="X2" s="7" t="s">
+      <c r="W2" s="4">
+        <v>0</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" s="7">
+      <c r="Y2" s="4">
         <v>60</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AA2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB2" s="7">
+      <c r="AA2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" s="4">
         <v>8</v>
       </c>
-      <c r="AC2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD2" s="7">
+      <c r="AC2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD2" s="4">
         <v>199</v>
       </c>
-      <c r="AE2" s="9">
+      <c r="AE2" s="6">
         <v>47.99</v>
       </c>
-      <c r="AF2" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="19">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="19">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="19">
+      <c r="AF2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
         <v>42099.25</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="5">
         <v>42106.25</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="4">
         <v>191189</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>3091519</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="5">
         <v>42089.73109872685</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="5">
         <v>42089.745022418982</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="5">
         <v>42100.535001851851</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="5">
         <v>42100.805278321757</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="5">
         <v>42089.731099108794</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R3" s="5">
         <v>42093.731099108794</v>
       </c>
-      <c r="S3" s="8">
+      <c r="S3" s="5">
         <v>42114.740296145836</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="7">
+      <c r="U3" s="4">
         <v>3</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="4">
         <v>5000</v>
       </c>
-      <c r="W3" s="7">
-        <v>0</v>
-      </c>
-      <c r="X3" s="7" t="s">
+      <c r="W3" s="4">
+        <v>0</v>
+      </c>
+      <c r="X3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Y3" s="7">
+      <c r="Y3" s="4">
         <v>60</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="Z3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB3" s="7">
+      <c r="AA3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB3" s="4">
         <v>8</v>
       </c>
-      <c r="AC3" s="7">
+      <c r="AC3" s="4">
         <v>5.5</v>
       </c>
-      <c r="AD3" s="7">
+      <c r="AD3" s="4">
         <v>199</v>
       </c>
-      <c r="AE3" s="9">
+      <c r="AE3" s="6">
         <v>47.99</v>
       </c>
-      <c r="AF3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="19">
-        <v>1</v>
-      </c>
-      <c r="AM3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="19">
-        <v>1</v>
-      </c>
-      <c r="AP3" s="19">
+      <c r="AF3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="15">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP3" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
         <v>42099.25</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="5">
         <v>42106.25</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>191205</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <v>3091547</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="5">
         <v>42103.560180439817</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="5">
         <v>42103.750712499997</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="5">
         <v>42103.740769594908</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="5">
         <v>42104.002542361108</v>
       </c>
-      <c r="Q4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" s="8">
+      <c r="Q4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="5">
         <v>42108.002542361108</v>
       </c>
-      <c r="S4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U4" s="7">
+      <c r="S4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" s="4">
         <v>4</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="4">
         <v>5000</v>
       </c>
-      <c r="W4" s="7">
+      <c r="W4" s="4">
         <v>634</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="X4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="Y4" s="4">
         <v>60</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="Z4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AA4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB4" s="7">
+      <c r="AA4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB4" s="4">
         <v>17</v>
       </c>
-      <c r="AC4" s="7">
+      <c r="AC4" s="4">
         <v>19.5</v>
       </c>
-      <c r="AD4" s="7">
+      <c r="AD4" s="4">
         <v>69</v>
       </c>
-      <c r="AE4" s="9">
+      <c r="AE4" s="6">
         <v>57</v>
       </c>
-      <c r="AF4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="19">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="19">
+      <c r="AF4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="15">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
         <v>42099.25</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
         <v>42106.25</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="4">
         <v>191206</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="4">
         <v>3091548</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="5">
         <v>42103.579953819448</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="5">
         <v>42103.632583483799</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="5">
         <v>42103.711877893518</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="5">
         <v>42103.961964120368</v>
       </c>
-      <c r="Q5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" s="8">
+      <c r="Q5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="5">
         <v>42107.961964120368</v>
       </c>
-      <c r="S5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U5" s="7">
+      <c r="S5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="4">
         <v>4</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="4">
         <v>5000</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="4">
         <v>790</v>
       </c>
-      <c r="X5" s="7" t="s">
+      <c r="X5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Y5" s="4">
         <v>60</v>
       </c>
-      <c r="Z5" s="7" t="s">
+      <c r="Z5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AA5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB5" s="7">
+      <c r="AA5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB5" s="4">
         <v>8</v>
       </c>
-      <c r="AC5" s="7">
+      <c r="AC5" s="4">
         <v>7</v>
       </c>
-      <c r="AD5" s="7">
+      <c r="AD5" s="4">
         <v>69</v>
       </c>
-      <c r="AE5" s="9">
+      <c r="AE5" s="6">
         <v>47.99</v>
       </c>
-      <c r="AF5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="19">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="19">
+      <c r="AF5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
         <v>42099.25</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="5">
         <v>42106.25</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>191207</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <v>3091539</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="5">
         <v>42097.547585729168</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="5">
         <v>42104.543095370369</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="5">
         <v>42105.584881168979</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="5">
         <v>42105.837185798613</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="Q6" s="5">
         <v>42097.547587349538</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="5">
         <v>42101.547587349538</v>
       </c>
-      <c r="S6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U6" s="7">
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" s="4">
         <v>4</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="4">
         <v>5000</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="4">
         <v>586</v>
       </c>
-      <c r="X6" s="7" t="s">
+      <c r="X6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Y6" s="4">
         <v>60</v>
       </c>
-      <c r="Z6" s="7" t="s">
+      <c r="Z6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AA6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB6" s="7">
+      <c r="AA6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB6" s="4">
         <v>8</v>
       </c>
-      <c r="AC6" s="7">
+      <c r="AC6" s="4">
         <v>3.5</v>
       </c>
-      <c r="AD6" s="7">
+      <c r="AD6" s="4">
         <v>69</v>
       </c>
-      <c r="AE6" s="9">
+      <c r="AE6" s="6">
         <v>47.99</v>
       </c>
-      <c r="AF6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="19">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="19">
-        <v>1</v>
-      </c>
-      <c r="AP6" s="19">
+      <c r="AF6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
         <v>42099.25</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <v>42106.25</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>191209</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>3091555</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="7" t="s">
+      <c r="G7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="5">
         <v>42105.561563113428</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="5">
         <v>42105.582905173615</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="5">
         <v>42105.71132642361</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="5">
         <v>42105.962375312498</v>
       </c>
-      <c r="Q7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R7" s="8">
+      <c r="Q7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R7" s="5">
         <v>42109.962375312498</v>
       </c>
-      <c r="S7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U7" s="7">
+      <c r="S7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="4">
         <v>4</v>
       </c>
-      <c r="V7" s="7">
+      <c r="V7" s="4">
         <v>5000</v>
       </c>
-      <c r="W7" s="7">
+      <c r="W7" s="4">
         <v>460</v>
       </c>
-      <c r="X7" s="7" t="s">
+      <c r="X7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="Y7" s="4">
         <v>60</v>
       </c>
-      <c r="Z7" s="7" t="s">
+      <c r="Z7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AA7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB7" s="7">
+      <c r="AA7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB7" s="4">
         <v>18</v>
       </c>
-      <c r="AC7" s="7">
+      <c r="AC7" s="4">
         <v>20</v>
       </c>
-      <c r="AD7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="9">
+      <c r="AD7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="6">
         <v>57.99</v>
       </c>
-      <c r="AF7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="19">
-        <v>1</v>
-      </c>
-      <c r="AJ7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="19">
-        <v>1</v>
-      </c>
-      <c r="AP7" s="19">
+      <c r="AF7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
         <v>42099.25</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="5">
         <v>42106.25</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="4">
         <v>191210</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="4">
         <v>3091556</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="G8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="5">
         <v>42105.687808564813</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="5">
         <v>42105.712052083334</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="5">
         <v>42105.915409837966</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8" s="5">
         <v>42106.165486458332</v>
       </c>
-      <c r="Q8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R8" s="8">
+      <c r="Q8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8" s="5">
         <v>42109.165486458332</v>
       </c>
-      <c r="S8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="T8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U8" s="7">
+      <c r="S8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U8" s="4">
         <v>4</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="4">
         <v>5000</v>
       </c>
-      <c r="W8" s="7">
-        <v>0</v>
-      </c>
-      <c r="X8" s="7" t="s">
+      <c r="W8" s="4">
+        <v>0</v>
+      </c>
+      <c r="X8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Y8" s="4">
         <v>60</v>
       </c>
-      <c r="Z8" s="7" t="s">
+      <c r="Z8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AA8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB8" s="7">
+      <c r="AA8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB8" s="4">
         <v>15</v>
       </c>
-      <c r="AC8" s="7">
+      <c r="AC8" s="4">
         <v>15</v>
       </c>
-      <c r="AD8" s="7">
+      <c r="AD8" s="4">
         <v>69</v>
       </c>
-      <c r="AE8" s="9">
+      <c r="AE8" s="6">
         <v>55.49</v>
       </c>
-      <c r="AF8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="19">
-        <v>1</v>
-      </c>
-      <c r="AJ8" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="19">
-        <v>1</v>
-      </c>
-      <c r="AP8" s="19">
+      <c r="AF8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="7">
         <v>2</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <v>42106.25</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>42113.25</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="7">
         <v>191211</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <v>3091541</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="7">
         <v>3</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="P9" s="11">
+      <c r="M9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="8">
         <v>42110.94199259259</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="Q9" s="8">
         <v>42110</v>
       </c>
-      <c r="R9" s="11">
+      <c r="R9" s="8">
         <v>42114</v>
       </c>
-      <c r="S9" s="11">
+      <c r="S9" s="8">
         <v>42114.71131716435</v>
       </c>
-      <c r="T9" s="10" t="s">
+      <c r="T9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="U9" s="10">
+      <c r="U9" s="7">
         <v>4</v>
       </c>
-      <c r="V9" s="10">
+      <c r="V9" s="7">
         <v>5000</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="7">
         <v>816</v>
       </c>
-      <c r="X9" s="10" t="s">
+      <c r="X9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Y9" s="7">
         <v>60</v>
       </c>
-      <c r="Z9" s="10" t="s">
+      <c r="Z9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AA9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB9" s="10">
+      <c r="AA9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB9" s="7">
         <v>16</v>
       </c>
-      <c r="AC9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="10">
+      <c r="AC9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1905,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,76 +1918,76 @@
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="9">
+      <c r="E2" s="6">
         <v>450</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="13">
         <v>42115.638426076388</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="4">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="E3" s="6">
         <v>500</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="13">
         <v>42115.638426076388</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="18"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="2">
         <f>SUM(E2:E4)</f>

</xml_diff>